<commit_message>
Removing rows without corps
</commit_message>
<xml_diff>
--- a/tests/data/expected_output.xlsx
+++ b/tests/data/expected_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="6880" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="5980" yWindow="560" windowWidth="27360" windowHeight="15880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>